<commit_message>
Added cusSlide.RT (instead of cusSlide.RESP as originally planned) and updated UCSB data column names.
</commit_message>
<xml_diff>
--- a/Data/UCSB-Social-Cue-2/test_data.xlsx
+++ b/Data/UCSB-Social-Cue-2/test_data.xlsx
@@ -7,8 +7,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="test-data.csv-1" sheetId="2" r:id="rId1"/>
-    <sheet name="test-data.csv" sheetId="1" r:id="rId2"/>
+    <sheet name="test-data.csv-2" sheetId="3" r:id="rId1"/>
+    <sheet name="test-data.csv-1" sheetId="2" r:id="rId2"/>
+    <sheet name="test-data.csv" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="131">
   <si>
     <t>ExperimentName</t>
   </si>
@@ -804,9 +805,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1000</v>
+      </c>
+      <c r="F2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>82</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1000</v>
+      </c>
+      <c r="F3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H3">
+        <v>392</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:I3"/>
     </sheetView>
   </sheetViews>
@@ -920,7 +1028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG3"/>
   <sheetViews>

</xml_diff>